<commit_message>
Update the code and results for the iterative method
</commit_message>
<xml_diff>
--- a/demo/Execution_Times_239375E.xlsx
+++ b/demo/Execution_Times_239375E.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofmora-my.sharepoint.com/personal/150699u_uom_lk/Documents/UoM-MSc-in-CS-2023/Semester-1/CS5229-Big-Data-Analytics-Technoogies/Assignments/UoM_MapReduce-vs-Spark/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="11_F25DC773A252ABDACC104866D15C67585ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4350841C-95BF-4829-8E3F-13A9360B02BD}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="11_F25DC773A252ABDACC104866D15C67585ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{723D732F-5C9C-4E5D-87BE-DDFCEA186B49}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-25470" yWindow="3315" windowWidth="17250" windowHeight="8865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Execution-Times" sheetId="1" r:id="rId1"/>
     <sheet name="Average-Execution-Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -330,20 +330,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>17.329999999999998</c:v>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>16.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.66</c:v>
+                  <c:v>1.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.02</c:v>
+                  <c:v>3.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.57</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>17.579999999999998</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -828,19 +828,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>20.7</c:v>
+                  <c:v>15.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.98</c:v>
+                  <c:v>1.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.37</c:v>
+                  <c:v>3.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.61</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19.05</c:v>
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1324,19 +1324,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>26.72</c:v>
+                  <c:v>15.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.71</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.329999999999998</c:v>
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.43</c:v>
+                  <c:v>1.1299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.13</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1820,19 +1820,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16.260000000000002</c:v>
+                  <c:v>19.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.77</c:v>
+                  <c:v>1.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.37</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.78</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.74</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2317,19 +2317,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>21.67</c:v>
+                  <c:v>20.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.22</c:v>
+                  <c:v>1.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.47</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.78</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21.02</c:v>
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2977,19 +2977,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19.031999999999996</c:v>
+                  <c:v>4.5920000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.141999999999999</c:v>
+                  <c:v>4.5860000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.231999999999999</c:v>
+                  <c:v>4.9639999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.863999999999997</c:v>
+                  <c:v>3.9339999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.184000000000001</c:v>
+                  <c:v>4.7839999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7579,8 +7579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7615,8 +7615,8 @@
       <c r="C2" s="6">
         <v>44.201999999999998</v>
       </c>
-      <c r="D2" s="3">
-        <v>17.329999999999998</v>
+      <c r="D2" s="6">
+        <v>16.8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -7628,7 +7628,7 @@
         <v>28.527000000000001</v>
       </c>
       <c r="D3" s="3">
-        <v>21.66</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -7640,7 +7640,7 @@
         <v>27.146000000000001</v>
       </c>
       <c r="D4" s="3">
-        <v>21.02</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -7652,7 +7652,7 @@
         <v>32.802</v>
       </c>
       <c r="D5" s="3">
-        <v>17.57</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -7664,7 +7664,7 @@
         <v>31.736999999999998</v>
       </c>
       <c r="D6" s="6">
-        <v>17.579999999999998</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -7678,7 +7678,7 @@
         <v>34.061999999999998</v>
       </c>
       <c r="D7" s="6">
-        <v>20.7</v>
+        <v>15.88</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -7690,7 +7690,7 @@
         <v>32.676000000000002</v>
       </c>
       <c r="D8" s="3">
-        <v>15.98</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -7702,7 +7702,7 @@
         <v>34.878</v>
       </c>
       <c r="D9" s="3">
-        <v>20.37</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -7714,7 +7714,7 @@
         <v>39.948999999999998</v>
       </c>
       <c r="D10" s="3">
-        <v>19.61</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -7725,8 +7725,8 @@
       <c r="C11" s="6">
         <v>32.61</v>
       </c>
-      <c r="D11" s="3">
-        <v>19.05</v>
+      <c r="D11" s="6">
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -7740,7 +7740,7 @@
         <v>31.001999999999999</v>
       </c>
       <c r="D12" s="3">
-        <v>21.67</v>
+        <v>20.79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -7752,7 +7752,7 @@
         <v>34.548000000000002</v>
       </c>
       <c r="D13" s="3">
-        <v>18.22</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -7764,7 +7764,7 @@
         <v>31.285</v>
       </c>
       <c r="D14" s="3">
-        <v>18.47</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -7776,7 +7776,7 @@
         <v>31.312000000000001</v>
       </c>
       <c r="D15" s="3">
-        <v>21.78</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -7787,8 +7787,8 @@
       <c r="C16" s="6">
         <v>31.678000000000001</v>
       </c>
-      <c r="D16" s="3">
-        <v>21.02</v>
+      <c r="D16" s="6">
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -7802,7 +7802,7 @@
         <v>34.476999999999997</v>
       </c>
       <c r="D17" s="3">
-        <v>26.72</v>
+        <v>15.31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -7814,7 +7814,7 @@
         <v>30.102</v>
       </c>
       <c r="D18" s="3">
-        <v>20.71</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -7825,8 +7825,8 @@
       <c r="C19" s="6">
         <v>33.826999999999998</v>
       </c>
-      <c r="D19" s="3">
-        <v>16.329999999999998</v>
+      <c r="D19" s="6">
+        <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -7838,7 +7838,7 @@
         <v>27.577999999999999</v>
       </c>
       <c r="D20" s="3">
-        <v>20.43</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -7850,7 +7850,7 @@
         <v>31.027000000000001</v>
       </c>
       <c r="D21" s="3">
-        <v>20.13</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -7864,7 +7864,7 @@
         <v>32.685000000000002</v>
       </c>
       <c r="D22" s="3">
-        <v>16.260000000000002</v>
+        <v>19.82</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -7876,7 +7876,7 @@
         <v>32.286999999999999</v>
       </c>
       <c r="D23" s="3">
-        <v>21.77</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -7888,7 +7888,7 @@
         <v>34.457999999999998</v>
       </c>
       <c r="D24" s="3">
-        <v>18.37</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -7900,7 +7900,7 @@
         <v>33.418999999999997</v>
       </c>
       <c r="D25" s="3">
-        <v>18.78</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -7912,7 +7912,7 @@
         <v>31.332000000000001</v>
       </c>
       <c r="D26" s="3">
-        <v>20.74</v>
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>
@@ -7964,7 +7964,7 @@
       </c>
       <c r="C2" s="7">
         <f>AVERAGE('Execution-Times'!D2:D6)</f>
-        <v>19.031999999999996</v>
+        <v>4.5920000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7977,7 +7977,7 @@
       </c>
       <c r="C3" s="7">
         <f>AVERAGE('Execution-Times'!D7:D11)</f>
-        <v>19.141999999999999</v>
+        <v>4.5860000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -7990,7 +7990,7 @@
       </c>
       <c r="C4" s="7">
         <f>AVERAGE('Execution-Times'!D12:D16)</f>
-        <v>20.231999999999999</v>
+        <v>4.9639999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="C5" s="7">
         <f>AVERAGE('Execution-Times'!D17:D21)</f>
-        <v>20.863999999999997</v>
+        <v>3.9339999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -8016,7 +8016,7 @@
       </c>
       <c r="C6" s="7">
         <f>AVERAGE('Execution-Times'!D22:D26)</f>
-        <v>19.184000000000001</v>
+        <v>4.7839999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>